<commit_message>
Minor fixes on Dining room
</commit_message>
<xml_diff>
--- a/Logic/MMM Items.xlsx
+++ b/Logic/MMM Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Unity\MMM\Assets\Logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5581C1-6638-406D-9BF8-B75A3A2C8199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37065775-5A9B-4096-93E5-059C2C5908FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9590" yWindow="2580" windowWidth="24900" windowHeight="17090" xr2:uid="{154F0FB3-9ECB-43D3-8599-B6AA6C81D68B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="117">
   <si>
     <t>Piano that can be played</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Shovel</t>
   </si>
   <si>
-    <t>Cape</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -356,6 +353,39 @@
   </si>
   <si>
     <t>Make the Meteor become an influencer star on Itchagram</t>
+  </si>
+  <si>
+    <t>Coat</t>
+  </si>
+  <si>
+    <t>Service room</t>
+  </si>
+  <si>
+    <t>Something for the woods, and probably also something extra to be decided</t>
+  </si>
+  <si>
+    <t>Shelf</t>
+  </si>
+  <si>
+    <t>Man eating plant</t>
+  </si>
+  <si>
+    <t>Can satisfy green tentacle</t>
+  </si>
+  <si>
+    <t>Can satisfy green tentacle, makes Ed going around if missing</t>
+  </si>
+  <si>
+    <t>Infirmary</t>
+  </si>
+  <si>
+    <t>Bathroom</t>
+  </si>
+  <si>
+    <t>Art room</t>
+  </si>
+  <si>
+    <t>Green tentacle room</t>
   </si>
 </sst>
 </file>
@@ -716,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6D92E7-76EF-47A2-BEF9-CB212DA98665}">
-  <dimension ref="B3:F87"/>
+  <dimension ref="B3:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,13 +761,13 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
@@ -745,13 +775,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -759,330 +789,411 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
         <v>69</v>
       </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
         <v>67</v>
       </c>
-      <c r="F6" t="s">
-        <v>80</v>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
+      <c r="C61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" t="s">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
+      <c r="C63" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" t="s">
+      <c r="C64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
+      <c r="C72" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
+      <c r="C75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" t="s">
+      <c r="C76" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
+      <c r="C77" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" t="s">
+      <c r="C78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>50</v>
-      </c>
-      <c r="C81" t="s">
-        <v>66</v>
-      </c>
-      <c r="D81" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B82" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B83" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="C84" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1106,175 +1217,175 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>